<commit_message>
[CPACS Reader, JSBSim] Code review and refactoring.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/CPACS/Matlab/comparison.xlsx
+++ b/JPADSandBox_v2/CPACS/Matlab/comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>C_D</t>
   </si>
@@ -143,9 +143,6 @@
     <t>aileron</t>
   </si>
   <si>
-    <t>in the CPACS defined until 3°, in JSBSim 40° (magnitude 0.04 in CPACS and 0.9 in JSBSim) same in outer flap</t>
-  </si>
-  <si>
     <t>elevator</t>
   </si>
   <si>
@@ -234,6 +231,12 @@
   </si>
   <si>
     <t>slightly lower 13%</t>
+  </si>
+  <si>
+    <t>in the CPACS defined until 3°, in JSBSim 40° (0.04 in CPACS (3°) and 0.9 (40°) in JSBSim) same in outer flap</t>
+  </si>
+  <si>
+    <t>invertire deltaA in flight gear</t>
   </si>
 </sst>
 </file>
@@ -591,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2F3792-C117-4B33-9B9F-0714A38FA0E0}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,10 +625,10 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -648,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -671,7 +674,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -694,7 +697,7 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -740,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -793,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -817,7 +820,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -843,7 +846,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -851,17 +854,17 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -869,34 +872,39 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
         <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
-        <v>45</v>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>